<commit_message>
finish the express and preemptable mix random test case
</commit_message>
<xml_diff>
--- a/VER/test_list.xlsx
+++ b/VER/test_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\tsn\VER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E961684C-E864-45B4-9B56-9271C67A23FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E44DC-01C0-47CB-A2AE-B5658A69173A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="8023BR" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>test_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +61,16 @@
   </si>
   <si>
     <t>3.simple_e_p_mix_packet_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.simple_e_p_mix_random_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;express packet and preemptable packet random 
+&gt;packet length of express  and  preemptable packet are both random
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -112,9 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -395,16 +409,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -440,6 +454,14 @@
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add register config class and rgm_user_seq
</commit_message>
<xml_diff>
--- a/VER/test_list.xlsx
+++ b/VER/test_list.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\tsn\VER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E44DC-01C0-47CB-A2AE-B5658A69173A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0984B4F-8402-424B-A183-D0556272C7D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="8023BR" sheetId="1" r:id="rId1"/>
+    <sheet name="background" sheetId="8" r:id="rId1"/>
+    <sheet name="1.basic case" sheetId="3" r:id="rId2"/>
+    <sheet name="2.throughput" sheetId="2" r:id="rId3"/>
+    <sheet name="3.8023BR" sheetId="1" r:id="rId4"/>
+    <sheet name="4.1588" sheetId="7" r:id="rId5"/>
+    <sheet name="5.8021QBV" sheetId="6" r:id="rId6"/>
+    <sheet name="performance" sheetId="5" r:id="rId7"/>
+    <sheet name="error_injection" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>test_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +83,192 @@
     <t xml:space="preserve">&gt;express packet and preemptable packet random 
 &gt;packet length of express  and  preemptable packet are both random
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出报文与输入报文完全一致，无丢包，无crc错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_ge_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_xge_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coverage point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_xge_ge_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任意xgmii 接口输入普通以太网报文，通过配置从相应GMII接口输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任意xgmii 接口输入普通以太网报文，通过配置从相应XGMII接口输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任意 gmii 接口输入普通以太网报文，通过配置从相应GMII接口输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_reg_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寄存器读写测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读出值与写入值一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从PCIE 接口输入普通以太网报文，通过配置从相应GMII接口输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从PCIE 接口输入普通以太网报文，通过配置从相应XGMII接口输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_pcie_ge_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_pcie_xge_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8x8 GE 配置随机交换，验证满流量二层交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coverage point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2XGE/8GE  配置随机交换，验证满流量二层交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>packet length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_ge_l2_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_xge_ge_l2_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_ge_vlan_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_xge_ge_vlan_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8x8 GE 配置随机交换，验证满流量基于VLAN交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2XGE/8GE  配置随机交换，验证满流量基于VLAN交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_xge_ge_mix_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2XGE/8GE  配置随机交换，验证满流量同时基于VLAN和L2交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input port x output port x packet length x (config?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_port_mix_switch_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCIE /2XGE/8GE  配置随机交换，验证满流量同时L2交换业务通路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并后报文比对一致，无丢包，无crc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并后报文和express报文各自比对一致，无丢包，无crc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>packet len x packet type x preempt count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1588报文收发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1588_packet_slave_rcv_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正确识别1588报文并按预回送报文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1588_packet_transparent_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>透明节点转发报文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正确修改报文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满流量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1， TSN 标准族</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前需支持的标准：
+1，IEEE 802.1Qbu/802.3br
+2，IEEE 802.1Qci
+3，IEEE 802.1Qbv
+4，IEEE 802.1Qav
+5，IEEE 802.1CB
+6，IEEE 802.1AS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -123,11 +321,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,6 +345,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>73084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6576908</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3676650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{955BE089-D4FF-4352-B314-B1BBFDB0C1A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="38100" y="435034"/>
+          <a:ext cx="6538808" cy="3603566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,60 +675,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7620FF-A5F2-40EC-AD79-0995FB1A7599}">
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.75" customWidth="1"/>
+    <col min="1" max="1" width="87" customWidth="1"/>
+    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="297.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665C8AE2-700D-4D3D-BFDE-E127EDED3C43}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.75" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1.6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79219B14-3ED5-4E54-BF46-4525C4844294}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2.1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2.2000000000000002</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2.2999999999999998</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -469,4 +1022,238 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.75" customWidth="1"/>
+    <col min="4" max="4" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3.1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCAF527-E3A0-459E-A92C-995B4825395B}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7855AF3-63D1-4FDA-BB44-BA48AA16A2BA}">
+  <dimension ref="B1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33FBEBA-D71A-4FCC-B54D-7BEF66F2F905}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47C4F3-D12E-430C-A767-E297962AF5FD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>